<commit_message>
remapping IO pins around unavailable IO on board. Steppers are still in progress
</commit_message>
<xml_diff>
--- a/GPIO Mapping.xlsx
+++ b/GPIO Mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t xml:space="preserve">Port A</t>
   </si>
@@ -37,13 +37,13 @@
     <t xml:space="preserve">Port D</t>
   </si>
   <si>
-    <t xml:space="preserve">Output 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caution – may be connected to PB_8</t>
+    <t xml:space="preserve">Remora Output 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Output 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_STEP</t>
   </si>
   <si>
     <t xml:space="preserve">14 inputs</t>
@@ -52,22 +52,16 @@
     <t xml:space="preserve">Z_STEP</t>
   </si>
   <si>
-    <t xml:space="preserve">Input 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caution – may be connected to PB_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 13</t>
+    <t xml:space="preserve">Remora Input 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_DIR</t>
   </si>
   <si>
     <t xml:space="preserve">8 outputs</t>
   </si>
   <si>
-    <t xml:space="preserve">Output 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 8</t>
+    <t xml:space="preserve">Remora Input 10</t>
   </si>
   <si>
     <t xml:space="preserve">B_STEP</t>
@@ -76,9 +70,6 @@
     <t xml:space="preserve">6 step generators</t>
   </si>
   <si>
-    <t xml:space="preserve">Output 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">C_STEP</t>
   </si>
   <si>
@@ -91,7 +82,10 @@
     <t xml:space="preserve">C_DIR</t>
   </si>
   <si>
-    <t xml:space="preserve">Output 7</t>
+    <t xml:space="preserve">Remora Output 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested working</t>
   </si>
   <si>
     <t xml:space="preserve">SPI1_CLK</t>
@@ -103,58 +97,64 @@
     <t xml:space="preserve">UART_RX</t>
   </si>
   <si>
+    <t xml:space="preserve">Tested – cannot get working</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPI1_MISO</t>
   </si>
   <si>
     <t xml:space="preserve">WIZ_CS</t>
   </si>
   <si>
-    <t xml:space="preserve">Input 2</t>
+    <t xml:space="preserve">Remora Input 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not yet yested</t>
   </si>
   <si>
     <t xml:space="preserve">SPI1_MOSI</t>
   </si>
   <si>
-    <t xml:space="preserve">Input 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caution – may be connected to PC_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caution – may be connected to PC_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 11</t>
+    <t xml:space="preserve">Remora Input 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Remora Input 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Output 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 13</t>
   </si>
   <si>
     <t xml:space="preserve">UART_TX</t>
   </si>
   <si>
-    <t xml:space="preserve">Input 4</t>
+    <t xml:space="preserve">Remora Input 6</t>
   </si>
   <si>
     <t xml:space="preserve">X_STEP</t>
   </si>
   <si>
-    <t xml:space="preserve">Input 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 5</t>
+    <t xml:space="preserve">Remora Input 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Input 7</t>
   </si>
   <si>
     <t xml:space="preserve">X_DIR</t>
@@ -163,25 +163,22 @@
     <t xml:space="preserve">DO NOT USE – SWD connection to STLink</t>
   </si>
   <si>
-    <t xml:space="preserve">A_STEP</t>
+    <t xml:space="preserve">Remora Output 4</t>
   </si>
   <si>
     <t xml:space="preserve">Y_STEP</t>
   </si>
   <si>
-    <t xml:space="preserve">A_DIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y_DIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input 12</t>
+    <t xml:space="preserve">Remora Output 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unusable unless LSE jumper cleared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Output 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remora Output 6</t>
   </si>
 </sst>
 </file>
@@ -226,7 +223,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,12 +232,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -290,6 +311,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -316,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,23 +365,59 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,15 +425,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,12 +498,12 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -452,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -462,7 +534,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,11 +576,11 @@
       <c r="E2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
@@ -517,143 +589,146 @@
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="10"/>
+      <c r="J3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="11"/>
       <c r="C4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
       <c r="J4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="11"/>
       <c r="C5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>21</v>
+      <c r="B6" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="J6" s="13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="J7" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="J8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -662,16 +737,16 @@
       <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="4" t="n">
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -683,7 +758,7 @@
       <c r="C10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="15" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="4" t="n">
@@ -692,8 +767,8 @@
       <c r="F10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -705,7 +780,7 @@
       <c r="C11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="4" t="n">
@@ -714,8 +789,8 @@
       <c r="F11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -736,8 +811,8 @@
       <c r="F12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -746,22 +821,22 @@
       <c r="B13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="4" t="n">
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -773,11 +848,11 @@
       <c r="E14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
@@ -789,7 +864,7 @@
       <c r="C15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="4" t="n">
@@ -798,8 +873,8 @@
       <c r="F15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
@@ -811,39 +886,39 @@
       <c r="C16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="9" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="E17" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="F17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Moved UART to use STLink default comms port, frees up 2x GPIO
</commit_message>
<xml_diff>
--- a/GPIO Mapping.xlsx
+++ b/GPIO Mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t xml:space="preserve">Port A</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">8 outputs</t>
   </si>
   <si>
+    <t xml:space="preserve">Nucleo Virtual Comm Port</t>
+  </si>
+  <si>
     <t xml:space="preserve">Remora Input 10</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
     <t xml:space="preserve">WIZ_RST</t>
   </si>
   <si>
-    <t xml:space="preserve">UART_RX</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tested – cannot get working</t>
   </si>
   <si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">Remora Input 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UART_TX</t>
   </si>
   <si>
     <t xml:space="preserve">Remora Input 6</t>
@@ -389,7 +386,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -525,7 +522,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -616,41 +613,45 @@
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="J4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
@@ -660,24 +661,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
       <c r="J6" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -685,20 +686,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="F7" s="10"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
       <c r="J7" s="14" t="s">
@@ -808,9 +807,7 @@
       <c r="E12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="F12" s="10"/>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
     </row>
@@ -819,7 +816,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -827,7 +824,7 @@
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
@@ -837,19 +834,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>12</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
@@ -859,19 +856,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>13</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>13</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
@@ -881,19 +878,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>14</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>14</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
@@ -903,19 +900,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="21" t="n">
         <v>15</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="19" t="n">
         <v>15</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" s="23"/>
       <c r="H17" s="24"/>

</xml_diff>

<commit_message>
Bug no longer reproducible with ZDir. excel mapping is now reflective of what works in software
</commit_message>
<xml_diff>
--- a/GPIO Mapping.xlsx
+++ b/GPIO Mapping.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Remora Output 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Tested working</t>
+    <t xml:space="preserve">Tested – working</t>
   </si>
   <si>
     <t xml:space="preserve">SPI1_CLK</t>
@@ -230,7 +230,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF999999"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
@@ -253,8 +253,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -341,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,10 +390,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,23 +410,23 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -500,7 +496,7 @@
       <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -522,7 +518,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -660,7 +656,7 @@
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="4" t="n">
@@ -677,7 +673,7 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -700,7 +696,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -720,12 +716,12 @@
       <c r="E8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>29</v>
       </c>
     </row>
@@ -757,7 +753,7 @@
       <c r="C10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="4" t="n">
@@ -779,7 +775,7 @@
       <c r="C11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="4" t="n">
@@ -833,7 +829,7 @@
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -889,33 +885,33 @@
       <c r="E16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="n">
+      <c r="A17" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="21" t="n">
+      <c r="C17" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="19" t="n">
+      <c r="E17" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updates to some testing, all GPIO and stepper pins now work. Yet to test ABC axis as I don't have any example GCode for it. will have to trust that 5 axis works for now
</commit_message>
<xml_diff>
--- a/GPIO Mapping.xlsx
+++ b/GPIO Mapping.xlsx
@@ -235,12 +235,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
@@ -249,6 +243,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -341,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,15 +366,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,7 +382,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,15 +390,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -430,11 +426,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,7 +514,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,11 +565,11 @@
       <c r="E2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
@@ -582,25 +578,25 @@
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="9"/>
       <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
@@ -609,7 +605,7 @@
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="4" t="n">
@@ -621,11 +617,11 @@
       <c r="E4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
       <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
@@ -634,46 +630,46 @@
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="J6" s="12" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="J6" s="11" t="s">
         <v>22</v>
       </c>
     </row>
@@ -693,10 +689,10 @@
       <c r="E7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="J7" s="13" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="J7" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -716,12 +712,12 @@
       <c r="E8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="J8" s="15" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="J8" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -732,16 +728,16 @@
       <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="4" t="n">
         <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -753,7 +749,7 @@
       <c r="C10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="4" t="n">
@@ -762,8 +758,8 @@
       <c r="F10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -775,7 +771,7 @@
       <c r="C11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="4" t="n">
@@ -784,8 +780,8 @@
       <c r="F11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -803,9 +799,9 @@
       <c r="E12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -814,22 +810,22 @@
       <c r="B13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="4" t="n">
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -841,11 +837,11 @@
       <c r="E14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
@@ -857,7 +853,7 @@
       <c r="C15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="4" t="n">
@@ -866,8 +862,8 @@
       <c r="F15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
@@ -879,39 +875,39 @@
       <c r="C16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="n">
+      <c r="A17" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="19" t="n">
+      <c r="C17" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E17" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>